<commit_message>
modified p03.ipynb and updated project log.md
</commit_message>
<xml_diff>
--- a/Project03/Stage02_OrderedList/Sprint_Sheet_1.xlsx
+++ b/Project03/Stage02_OrderedList/Sprint_Sheet_1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darienyang/Documents/2018FALL/SSW-555/Project/repo/Project03/Stage02_OrderedList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D296737C-EDDF-C546-BB4D-248CD19454A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F4AD4239-B032-E74E-BA06-C96BDAAE4CC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3820" yWindow="-19160" windowWidth="28800" windowHeight="17560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -288,12 +288,6 @@
     <t>Corresponding entries</t>
   </si>
   <si>
-    <t>US27</t>
-  </si>
-  <si>
-    <t>Include individual ages</t>
-  </si>
-  <si>
     <t>US28</t>
   </si>
   <si>
@@ -328,6 +322,12 @@
   </si>
   <si>
     <t>https://github.com/SSW-555-Project/projectRepo</t>
+  </si>
+  <si>
+    <t>US33</t>
+  </si>
+  <si>
+    <t>List orphans</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -876,7 +876,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -885,7 +885,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1848,10 +1848,10 @@
     <row r="28" spans="1:26">
       <c r="A28" s="3"/>
       <c r="B28" s="6" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1880,10 +1880,10 @@
     <row r="29" spans="1:26">
       <c r="A29" s="3"/>
       <c r="B29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1912,10 +1912,10 @@
     <row r="30" spans="1:26">
       <c r="A30" s="3"/>
       <c r="B30" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1944,10 +1944,10 @@
     <row r="31" spans="1:26">
       <c r="A31" s="3"/>
       <c r="B31" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1976,10 +1976,10 @@
     <row r="32" spans="1:26">
       <c r="A32" s="3"/>
       <c r="B32" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2008,10 +2008,10 @@
     <row r="33" spans="1:26">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>

</xml_diff>